<commit_message>
report-poster: Add poster and presentation files
</commit_message>
<xml_diff>
--- a/experiments/illuminance vs angle/illuminance vs angle.xlsx
+++ b/experiments/illuminance vs angle/illuminance vs angle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="10% brightness" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,7 @@
     <sheet name="Blue" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="distance and illuminance" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Sheet10" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Sheet11" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -129,7 +130,7 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -177,7 +178,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -191,6 +192,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,7 +224,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -253,7 +258,7 @@
       <rgbColor rgb="FFED7D31"/>
       <rgbColor rgb="FF595959"/>
       <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -667,13 +672,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2239662"/>
-        <c:axId val="71286320"/>
+        <c:axId val="91987216"/>
+        <c:axId val="87367474"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="2239662"/>
+        <c:axId val="91987216"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -704,14 +709,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71286320"/>
+        <c:crossAx val="87367474"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71286320"/>
+        <c:axId val="87367474"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,7 +759,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2239662"/>
+        <c:crossAx val="91987216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -832,10 +837,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.128655405908178"/>
-          <c:y val="0.194933053294828"/>
-          <c:w val="0.871046952898281"/>
-          <c:h val="0.720661590968758"/>
+          <c:x val="0.128621089223638"/>
+          <c:y val="0.19495864513588"/>
+          <c:w val="0.871016801853998"/>
+          <c:h val="0.720624917946698"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1164,11 +1169,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="33397706"/>
-        <c:axId val="2957158"/>
+        <c:axId val="59022701"/>
+        <c:axId val="7503481"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="33397706"/>
+        <c:axId val="59022701"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,14 +1209,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2957158"/>
+        <c:crossAx val="7503481"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2957158"/>
+        <c:axId val="7503481"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1259,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33397706"/>
+        <c:crossAx val="59022701"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1683,13 +1688,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="24934930"/>
-        <c:axId val="53966527"/>
+        <c:axId val="58917814"/>
+        <c:axId val="58111571"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="24934930"/>
+        <c:axId val="58917814"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1720,14 +1725,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53966527"/>
+        <c:crossAx val="58111571"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53966527"/>
+        <c:axId val="58111571"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1770,7 +1775,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24934930"/>
+        <c:crossAx val="58917814"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2223,13 +2228,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="33000442"/>
-        <c:axId val="53759125"/>
+        <c:axId val="86405712"/>
+        <c:axId val="26044913"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="33000442"/>
+        <c:axId val="86405712"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2260,14 +2265,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53759125"/>
+        <c:crossAx val="26044913"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53759125"/>
+        <c:axId val="26044913"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2310,7 +2315,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33000442"/>
+        <c:crossAx val="86405712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2348,257 +2353,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'distance and illuminance'!$R$7:$R$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'distance and illuminance'!$S$7:$S$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.640774825533513</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4106698404076</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.292089969978291</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.217297297656968</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.165954718831698</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.131708062871185</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.111408068626885</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0891809067125453</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="58198428"/>
-        <c:axId val="55644757"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="58198428"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="55644757"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="55644757"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="58198428"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2610,9 +2364,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>344160</xdr:colOff>
+      <xdr:colOff>343800</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2620,8 +2374,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7593480" y="1023840"/>
-        <a:ext cx="4837680" cy="2741760"/>
+        <a:off x="7803000" y="1023840"/>
+        <a:ext cx="4970880" cy="2741400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2645,9 +2399,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>451440</xdr:colOff>
+      <xdr:colOff>451080</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2655,8 +2409,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14015880" y="1795320"/>
-        <a:ext cx="4837680" cy="2742120"/>
+        <a:off x="14397120" y="1795320"/>
+        <a:ext cx="4970520" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2680,9 +2434,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>208800</xdr:colOff>
+      <xdr:colOff>208440</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2690,8 +2444,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9124920" y="4376160"/>
-        <a:ext cx="4837680" cy="2742120"/>
+        <a:off x="9353520" y="4376160"/>
+        <a:ext cx="4970880" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2715,9 +2469,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>142560</xdr:colOff>
+      <xdr:colOff>142200</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>117720</xdr:rowOff>
+      <xdr:rowOff>117360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2725,43 +2479,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3472560" y="2371320"/>
-        <a:ext cx="5356800" cy="3537360"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>45000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>-7920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>115200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="14960880" y="-7920"/>
-        <a:ext cx="5870880" cy="3239280"/>
+        <a:off x="3548880" y="2371320"/>
+        <a:ext cx="5508720" cy="3537000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2782,15 +2501,15 @@
   <dimension ref="B5:N37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="K8:Q17 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4084,12 +3803,12 @@
   <dimension ref="B9:U22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="1" sqref="K8:Q17 F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4579,6 +4298,142 @@
       </c>
       <c r="U22" s="0" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B6:I45"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I37" activeCellId="1" sqref="K8:Q17 I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5023255813953"/>
+  </cols>
+  <sheetData>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="n">
+        <v>-90</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>-60</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>-30</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I37" s="4" t="n">
+        <f aca="false">'100% brightness'!F8</f>
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I38" s="4" t="n">
+        <f aca="false">'100% brightness'!F9</f>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="I39" s="4" t="n">
+        <f aca="false">'100% brightness'!F10</f>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I40" s="4" t="n">
+        <f aca="false">'100% brightness'!F11</f>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="I41" s="4" t="n">
+        <f aca="false">'100% brightness'!F12</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="I42" s="4" t="n">
+        <f aca="false">'100% brightness'!F13</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="I43" s="4" t="n">
+        <f aca="false">'100% brightness'!F14</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="I44" s="4" t="n">
+        <f aca="false">'100% brightness'!F15</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="I45" s="4" t="n">
+        <f aca="false">'100% brightness'!F16</f>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -4600,13 +4455,13 @@
   <dimension ref="B5:N37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="K8:Q17 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5734,13 +5589,13 @@
   <dimension ref="B5:N37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="K8:Q17 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7033,13 +6888,13 @@
   <dimension ref="B5:N37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="K8:Q17 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8157,14 +8012,14 @@
   </sheetPr>
   <dimension ref="B5:X37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="K8:Q17 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9602,12 +9457,12 @@
   <dimension ref="B22:N48"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="B40" activeCellId="1" sqref="K8:Q17 B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10393,12 +10248,12 @@
   <dimension ref="B6:N11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="K8:Q17 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10715,15 +10570,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C6:L28"/>
+  <dimension ref="C6:Q28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8:Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10768,6 +10623,34 @@
       <c r="G8" s="0" t="n">
         <v>2600</v>
       </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">G8</f>
+        <v>2600</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <f aca="false">F8</f>
+        <v>4840</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false">E8</f>
+        <v>4200</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <f aca="false">D8</f>
+        <v>4285</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <f aca="false">E8</f>
+        <v>4200</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <f aca="false">F8</f>
+        <v>4840</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <f aca="false">G8</f>
+        <v>2600</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="n">
@@ -10785,6 +10668,34 @@
       <c r="G9" s="0" t="n">
         <v>1998</v>
       </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">G9</f>
+        <v>1998</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <f aca="false">F9</f>
+        <v>5310</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <f aca="false">E9</f>
+        <v>5950</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <f aca="false">D9</f>
+        <v>6420</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <f aca="false">E9</f>
+        <v>5950</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <f aca="false">F9</f>
+        <v>5310</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <f aca="false">G9</f>
+        <v>1998</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="n">
@@ -10802,6 +10713,34 @@
       <c r="G10" s="0" t="n">
         <v>547</v>
       </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">G10</f>
+        <v>547</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <f aca="false">F10</f>
+        <v>3302</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">E10</f>
+        <v>3770</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <f aca="false">D10</f>
+        <v>4910</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <f aca="false">E10</f>
+        <v>3770</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <f aca="false">F10</f>
+        <v>3302</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <f aca="false">G10</f>
+        <v>547</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="n">
@@ -10819,6 +10758,34 @@
       <c r="G11" s="0" t="n">
         <v>149</v>
       </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">G11</f>
+        <v>149</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <f aca="false">F11</f>
+        <v>1657</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <f aca="false">E11</f>
+        <v>2354</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <f aca="false">D11</f>
+        <v>2507</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <f aca="false">E11</f>
+        <v>2354</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <f aca="false">F11</f>
+        <v>1657</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <f aca="false">G11</f>
+        <v>149</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="n">
@@ -10836,6 +10803,34 @@
       <c r="G12" s="0" t="n">
         <v>110</v>
       </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">G12</f>
+        <v>110</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <f aca="false">F12</f>
+        <v>1219</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <f aca="false">E12</f>
+        <v>1620</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <f aca="false">D12</f>
+        <v>1820</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <f aca="false">E12</f>
+        <v>1620</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <f aca="false">F12</f>
+        <v>1219</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <f aca="false">G12</f>
+        <v>110</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="n">
@@ -10853,6 +10848,34 @@
       <c r="G13" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">G13</f>
+        <v>60</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">F13</f>
+        <v>892</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <f aca="false">E13</f>
+        <v>1227</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <f aca="false">D13</f>
+        <v>1375</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <f aca="false">E13</f>
+        <v>1227</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <f aca="false">F13</f>
+        <v>892</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <f aca="false">G13</f>
+        <v>60</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="n">
@@ -10870,6 +10893,34 @@
       <c r="G14" s="0" t="n">
         <v>55</v>
       </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">G14</f>
+        <v>55</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">F14</f>
+        <v>691</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <f aca="false">E14</f>
+        <v>943</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">D14</f>
+        <v>1012</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <f aca="false">E14</f>
+        <v>943</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <f aca="false">F14</f>
+        <v>691</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">G14</f>
+        <v>55</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="n">
@@ -10887,6 +10938,34 @@
       <c r="G15" s="0" t="n">
         <v>43</v>
       </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">G15</f>
+        <v>43</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">F15</f>
+        <v>547</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <f aca="false">E15</f>
+        <v>785</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">D15</f>
+        <v>810</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <f aca="false">E15</f>
+        <v>785</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <f aca="false">F15</f>
+        <v>547</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">G15</f>
+        <v>43</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="n">
@@ -10904,6 +10983,34 @@
       <c r="G16" s="0" t="n">
         <v>35</v>
       </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">G16</f>
+        <v>35</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">F16</f>
+        <v>420</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <f aca="false">E16</f>
+        <v>607</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">D16</f>
+        <v>667</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <f aca="false">E16</f>
+        <v>607</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <f aca="false">F16</f>
+        <v>420</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <f aca="false">G16</f>
+        <v>35</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="n">
@@ -10919,6 +11026,34 @@
         <v>353</v>
       </c>
       <c r="G17" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">G17</f>
+        <v>30</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <f aca="false">F17</f>
+        <v>353</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <f aca="false">E17</f>
+        <v>500</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <f aca="false">D17</f>
+        <v>557</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <f aca="false">E17</f>
+        <v>500</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <f aca="false">F17</f>
+        <v>353</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <f aca="false">G17</f>
         <v>30</v>
       </c>
     </row>
@@ -11314,13 +11449,13 @@
   </sheetPr>
   <dimension ref="B5:T39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="1" sqref="K8:Q17 C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12969,6 +13104,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>